<commit_message>
Implements #1 - Add Javascript and C#
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -10,8 +10,11 @@
     <sheet name="stats.xlsx.csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_2015" localSheetId="0">stats.xlsx.csv!$N$2:$Y$6</definedName>
-    <definedName name="_2016" localSheetId="0">stats.xlsx.csv!$Z$2:$AI$6</definedName>
+    <definedName name="_2014__1" localSheetId="0">stats.xlsx.csv!#REF!</definedName>
+    <definedName name="_2015" localSheetId="0">stats.xlsx.csv!$N$2:$Y$8</definedName>
+    <definedName name="_2015__1" localSheetId="0">stats.xlsx.csv!#REF!</definedName>
+    <definedName name="_2016" localSheetId="0">stats.xlsx.csv!$Z$2:$AI$8</definedName>
+    <definedName name="_2016__1" localSheetId="0">stats.xlsx.csv!#REF!</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -24,8 +27,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="2015.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="Macintosh HD:Users:ekeller:Downloads:2015.csv" decimal="," thousands=" ">
+  <connection id="1" name="2014 (1).csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:ekeller:Downloads:2014 (1).csv" decimal="," thousands=" ">
       <textFields count="13">
         <textField/>
         <textField/>
@@ -43,7 +46,26 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="2016.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="2" name="2015.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:ekeller:Downloads:2015.csv" decimal="," thousands=" ">
+      <textFields count="13">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="2016.csv" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:ekeller:Downloads:2016.csv" decimal="," thousands=" ">
       <textFields count="13">
         <textField/>
@@ -66,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>C++</t>
   </si>
@@ -81,6 +103,12 @@
   </si>
   <si>
     <t>Swift</t>
+  </si>
+  <si>
+    <t>c#</t>
+  </si>
+  <si>
+    <t>Javascript</t>
   </si>
 </sst>
 </file>
@@ -132,8 +160,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -143,11 +183,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="17">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,7 +477,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Java</c:v>
+                  <c:v>c#</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -551,106 +603,106 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>20766.0</c:v>
+                  <c:v>4771.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21414.0</c:v>
+                  <c:v>4713.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26178.0</c:v>
+                  <c:v>5680.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26748.0</c:v>
+                  <c:v>5926.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29169.0</c:v>
+                  <c:v>6696.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26278.0</c:v>
+                  <c:v>6445.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26420.0</c:v>
+                  <c:v>6567.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26041.0</c:v>
+                  <c:v>6633.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31238.0</c:v>
+                  <c:v>7795.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36233.0</c:v>
+                  <c:v>8916.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>38825.0</c:v>
+                  <c:v>9217.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>38814.0</c:v>
+                  <c:v>9576.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>40639.0</c:v>
+                  <c:v>10627.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>39273.0</c:v>
+                  <c:v>10058.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>66473.0</c:v>
+                  <c:v>17199.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>61641.0</c:v>
+                  <c:v>15441.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>62018.0</c:v>
+                  <c:v>16112.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>58580.0</c:v>
+                  <c:v>14822.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>54329.0</c:v>
+                  <c:v>14257.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>54980.0</c:v>
+                  <c:v>14418.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>61126.0</c:v>
+                  <c:v>15281.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>69324.0</c:v>
+                  <c:v>17759.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>72593.0</c:v>
+                  <c:v>18313.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>71850.0</c:v>
+                  <c:v>18731.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>72445.0</c:v>
+                  <c:v>19708.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>80629.0</c:v>
+                  <c:v>20986.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>103005.0</c:v>
+                  <c:v>23545.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>104095.0</c:v>
+                  <c:v>25404.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>101442.0</c:v>
+                  <c:v>25997.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>96881.0</c:v>
+                  <c:v>25417.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>92797.0</c:v>
+                  <c:v>23844.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>102902.0</c:v>
+                  <c:v>25884.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>124221.0</c:v>
+                  <c:v>30700.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>157682.0</c:v>
+                  <c:v>40536.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -666,7 +718,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Go</c:v>
+                  <c:v>Java</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -792,106 +844,106 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>1232.0</c:v>
+                  <c:v>20766.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1221.0</c:v>
+                  <c:v>21414.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1400.0</c:v>
+                  <c:v>26178.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1508.0</c:v>
+                  <c:v>26748.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1670.0</c:v>
+                  <c:v>29169.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1623.0</c:v>
+                  <c:v>26278.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2012.0</c:v>
+                  <c:v>26420.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2088.0</c:v>
+                  <c:v>26041.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2204.0</c:v>
+                  <c:v>31238.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2190.0</c:v>
+                  <c:v>36233.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2283.0</c:v>
+                  <c:v>38825.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2528.0</c:v>
+                  <c:v>38814.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2903.0</c:v>
+                  <c:v>40639.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2767.0</c:v>
+                  <c:v>39273.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3586.0</c:v>
+                  <c:v>66473.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3283.0</c:v>
+                  <c:v>61641.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3427.0</c:v>
+                  <c:v>62018.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3331.0</c:v>
+                  <c:v>58580.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3546.0</c:v>
+                  <c:v>54329.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3762.0</c:v>
+                  <c:v>54980.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4118.0</c:v>
+                  <c:v>61126.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4417.0</c:v>
+                  <c:v>69324.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4418.0</c:v>
+                  <c:v>72593.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4547.0</c:v>
+                  <c:v>71850.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5044.0</c:v>
+                  <c:v>72445.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5077.0</c:v>
+                  <c:v>80629.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6222.0</c:v>
+                  <c:v>103005.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6233.0</c:v>
+                  <c:v>104095.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6377.0</c:v>
+                  <c:v>101442.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6354.0</c:v>
+                  <c:v>96881.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>6692.0</c:v>
+                  <c:v>92797.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8076.0</c:v>
+                  <c:v>102902.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>9309.0</c:v>
+                  <c:v>124221.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>11895.0</c:v>
+                  <c:v>157682.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -907,7 +959,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rust</c:v>
+                  <c:v>Javascript</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1033,106 +1085,106 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>112.0</c:v>
+                  <c:v>24710.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80.0</c:v>
+                  <c:v>27288.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>77.0</c:v>
+                  <c:v>30718.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>31468.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>124.0</c:v>
+                  <c:v>33339.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>117.0</c:v>
+                  <c:v>32029.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>169.0</c:v>
+                  <c:v>36225.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>185.0</c:v>
+                  <c:v>35706.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>146.0</c:v>
+                  <c:v>37123.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>238.0</c:v>
+                  <c:v>42169.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>303.0</c:v>
+                  <c:v>42299.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>313.0</c:v>
+                  <c:v>42081.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>423.0</c:v>
+                  <c:v>47234.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>336.0</c:v>
+                  <c:v>46948.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>399.0</c:v>
+                  <c:v>54630.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>421.0</c:v>
+                  <c:v>54132.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>747.0</c:v>
+                  <c:v>56344.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>612.0</c:v>
+                  <c:v>57247.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>609.0</c:v>
+                  <c:v>59390.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>592.0</c:v>
+                  <c:v>59881.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>616.0</c:v>
+                  <c:v>63032.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>600.0</c:v>
+                  <c:v>68212.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>625.0</c:v>
+                  <c:v>69975.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>717.0</c:v>
+                  <c:v>70520.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>925.0</c:v>
+                  <c:v>80083.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>826.0</c:v>
+                  <c:v>89816.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1065.0</c:v>
+                  <c:v>101852.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1063.0</c:v>
+                  <c:v>104463.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1285.0</c:v>
+                  <c:v>108099.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1323.0</c:v>
+                  <c:v>107482.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1285.0</c:v>
+                  <c:v>110806.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1568.0</c:v>
+                  <c:v>125817.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1755.0</c:v>
+                  <c:v>143704.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2495.0</c:v>
+                  <c:v>186834.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1148,7 +1200,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Swift</c:v>
+                  <c:v>Go</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1274,111 +1326,593 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>1232.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>1221.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>1400.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>1508.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>1670.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1005.0</c:v>
+                  <c:v>1623.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>942.0</c:v>
+                  <c:v>2012.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1077.0</c:v>
+                  <c:v>2088.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2343.0</c:v>
+                  <c:v>2204.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2777.0</c:v>
+                  <c:v>2190.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2512.0</c:v>
+                  <c:v>2283.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2344.0</c:v>
+                  <c:v>2528.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2864.0</c:v>
+                  <c:v>2903.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3079.0</c:v>
+                  <c:v>2767.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3699.0</c:v>
+                  <c:v>3586.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4242.0</c:v>
+                  <c:v>3283.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4252.0</c:v>
+                  <c:v>3427.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4542.0</c:v>
+                  <c:v>3331.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4362.0</c:v>
+                  <c:v>3546.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4376.0</c:v>
+                  <c:v>3762.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5256.0</c:v>
+                  <c:v>4118.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6511.0</c:v>
+                  <c:v>4417.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6753.0</c:v>
+                  <c:v>4418.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7366.0</c:v>
+                  <c:v>4547.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8377.0</c:v>
+                  <c:v>5044.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9948.0</c:v>
+                  <c:v>5077.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>10328.0</c:v>
+                  <c:v>6222.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9846.0</c:v>
+                  <c:v>6233.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>10042.0</c:v>
+                  <c:v>6377.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>10403.0</c:v>
+                  <c:v>6354.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>10474.0</c:v>
+                  <c:v>6692.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>10832.0</c:v>
+                  <c:v>8076.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>13832.0</c:v>
+                  <c:v>9309.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>17213.0</c:v>
+                  <c:v>11895.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stats.xlsx.csv!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rust</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$1:$AI$1</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>40178.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40209.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40237.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40268.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40298.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40329.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40359.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40390.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40421.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40451.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40482.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40512.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40543.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40574.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40602.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40633.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40663.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40694.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40755.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40786.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40816.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40847.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40877.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40908.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40939.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40968.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40999.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41029.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41060.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41090.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41121.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41152.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41182.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$7:$AI$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>112.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>117.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>169.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>185.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>146.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>238.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>303.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>313.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>423.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>336.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>399.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>421.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>747.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>612.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>609.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>592.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>616.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>625.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>717.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>925.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>826.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1065.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1063.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1285.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1323.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1285.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1568.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1755.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2495.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stats.xlsx.csv!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Swift</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$1:$AI$1</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>40178.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40209.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40237.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40268.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40298.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40329.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40359.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40390.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40421.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40451.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40482.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40512.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40543.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40574.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40602.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40633.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40663.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40694.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40755.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40786.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40816.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40847.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40877.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40908.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40939.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40968.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40999.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41029.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41060.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41090.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41121.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41152.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41182.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$8:$AI$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1005.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>942.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1077.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2343.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2777.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2512.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2344.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2864.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3079.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3699.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4242.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4252.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4542.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4362.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4376.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5256.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6511.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6753.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7366.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8377.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9948.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10328.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9846.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10042.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10403.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10474.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>10832.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>13832.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>17213.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1390,11 +1924,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2115374024"/>
-        <c:axId val="2115400888"/>
+        <c:axId val="2124205672"/>
+        <c:axId val="2124208856"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2115374024"/>
+        <c:axId val="2124205672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1414,14 +1948,14 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115400888"/>
+        <c:crossAx val="2124208856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2115400888"/>
+        <c:axId val="2124208856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1443,7 +1977,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115374024"/>
+        <c:crossAx val="2124205672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1454,9 +1988,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.123981418412664"/>
+          <c:x val="0.0582374737759856"/>
           <c:y val="0.0132669983416252"/>
-          <c:w val="0.700133958168724"/>
+          <c:w val="0.941762526224014"/>
           <c:h val="0.0533429963045664"/>
         </c:manualLayout>
       </c:layout>
@@ -1490,13 +2024,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1520,11 +2054,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2015" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2016" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2016" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2015" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1849,15 +2383,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI6"/>
+  <dimension ref="A1:AI8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y28" sqref="Y28"/>
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
@@ -1884,14 +2418,13 @@
     <col min="25" max="25" width="7" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="6.5" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.1640625" customWidth="1"/>
+    <col min="28" max="29" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6.1640625" customWidth="1"/>
-    <col min="33" max="33" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="7.1640625" customWidth="1"/>
-    <col min="35" max="35" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.1640625" customWidth="1"/>
+    <col min="33" max="35" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="7.1640625" customWidth="1"/>
+    <col min="38" max="38" width="2.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -2107,429 +2640,643 @@
     </row>
     <row r="3" spans="1:35">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>20766</v>
+        <v>4771</v>
       </c>
       <c r="C3">
-        <v>21414</v>
+        <v>4713</v>
       </c>
       <c r="D3">
-        <v>26178</v>
+        <v>5680</v>
       </c>
       <c r="E3">
-        <v>26748</v>
+        <v>5926</v>
       </c>
       <c r="F3">
-        <v>29169</v>
+        <v>6696</v>
       </c>
       <c r="G3">
-        <v>26278</v>
+        <v>6445</v>
       </c>
       <c r="H3">
-        <v>26420</v>
+        <v>6567</v>
       </c>
       <c r="I3">
-        <v>26041</v>
+        <v>6633</v>
       </c>
       <c r="J3">
-        <v>31238</v>
+        <v>7795</v>
       </c>
       <c r="K3">
-        <v>36233</v>
+        <v>8916</v>
       </c>
       <c r="L3">
-        <v>38825</v>
+        <v>9217</v>
       </c>
       <c r="M3">
-        <v>38814</v>
+        <v>9576</v>
       </c>
       <c r="N3">
-        <v>40639</v>
+        <v>10627</v>
       </c>
       <c r="O3">
-        <v>39273</v>
+        <v>10058</v>
       </c>
       <c r="P3">
-        <v>66473</v>
+        <v>17199</v>
       </c>
       <c r="Q3">
-        <v>61641</v>
+        <v>15441</v>
       </c>
       <c r="R3">
-        <v>62018</v>
+        <v>16112</v>
       </c>
       <c r="S3">
-        <v>58580</v>
+        <v>14822</v>
       </c>
       <c r="T3">
-        <v>54329</v>
+        <v>14257</v>
       </c>
       <c r="U3">
-        <v>54980</v>
+        <v>14418</v>
       </c>
       <c r="V3">
-        <v>61126</v>
+        <v>15281</v>
       </c>
       <c r="W3">
-        <v>69324</v>
+        <v>17759</v>
       </c>
       <c r="X3">
-        <v>72593</v>
+        <v>18313</v>
       </c>
       <c r="Y3">
-        <v>71850</v>
+        <v>18731</v>
       </c>
       <c r="Z3">
-        <v>72445</v>
+        <v>19708</v>
       </c>
       <c r="AA3">
-        <v>80629</v>
+        <v>20986</v>
       </c>
       <c r="AB3">
-        <v>103005</v>
+        <v>23545</v>
       </c>
       <c r="AC3">
-        <v>104095</v>
+        <v>25404</v>
       </c>
       <c r="AD3">
-        <v>101442</v>
+        <v>25997</v>
       </c>
       <c r="AE3">
-        <v>96881</v>
+        <v>25417</v>
       </c>
       <c r="AF3">
-        <v>92797</v>
+        <v>23844</v>
       </c>
       <c r="AG3">
-        <v>102902</v>
+        <v>25884</v>
       </c>
       <c r="AH3">
-        <v>124221</v>
+        <v>30700</v>
       </c>
       <c r="AI3">
-        <v>157682</v>
+        <v>40536</v>
       </c>
     </row>
     <row r="4" spans="1:35">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>1232</v>
+        <v>20766</v>
       </c>
       <c r="C4">
-        <v>1221</v>
+        <v>21414</v>
       </c>
       <c r="D4">
-        <v>1400</v>
+        <v>26178</v>
       </c>
       <c r="E4">
-        <v>1508</v>
+        <v>26748</v>
       </c>
       <c r="F4">
-        <v>1670</v>
+        <v>29169</v>
       </c>
       <c r="G4">
-        <v>1623</v>
+        <v>26278</v>
       </c>
       <c r="H4">
-        <v>2012</v>
+        <v>26420</v>
       </c>
       <c r="I4">
-        <v>2088</v>
+        <v>26041</v>
       </c>
       <c r="J4">
-        <v>2204</v>
+        <v>31238</v>
       </c>
       <c r="K4">
-        <v>2190</v>
+        <v>36233</v>
       </c>
       <c r="L4">
-        <v>2283</v>
+        <v>38825</v>
       </c>
       <c r="M4">
-        <v>2528</v>
+        <v>38814</v>
       </c>
       <c r="N4">
-        <v>2903</v>
+        <v>40639</v>
       </c>
       <c r="O4">
-        <v>2767</v>
+        <v>39273</v>
       </c>
       <c r="P4">
-        <v>3586</v>
+        <v>66473</v>
       </c>
       <c r="Q4">
-        <v>3283</v>
+        <v>61641</v>
       </c>
       <c r="R4">
-        <v>3427</v>
+        <v>62018</v>
       </c>
       <c r="S4">
-        <v>3331</v>
+        <v>58580</v>
       </c>
       <c r="T4">
-        <v>3546</v>
+        <v>54329</v>
       </c>
       <c r="U4">
-        <v>3762</v>
+        <v>54980</v>
       </c>
       <c r="V4">
-        <v>4118</v>
+        <v>61126</v>
       </c>
       <c r="W4">
-        <v>4417</v>
+        <v>69324</v>
       </c>
       <c r="X4">
-        <v>4418</v>
+        <v>72593</v>
       </c>
       <c r="Y4">
-        <v>4547</v>
+        <v>71850</v>
       </c>
       <c r="Z4">
-        <v>5044</v>
+        <v>72445</v>
       </c>
       <c r="AA4">
-        <v>5077</v>
+        <v>80629</v>
       </c>
       <c r="AB4">
-        <v>6222</v>
+        <v>103005</v>
       </c>
       <c r="AC4">
-        <v>6233</v>
+        <v>104095</v>
       </c>
       <c r="AD4">
-        <v>6377</v>
+        <v>101442</v>
       </c>
       <c r="AE4">
-        <v>6354</v>
+        <v>96881</v>
       </c>
       <c r="AF4">
-        <v>6692</v>
+        <v>92797</v>
       </c>
       <c r="AG4">
-        <v>8076</v>
+        <v>102902</v>
       </c>
       <c r="AH4">
-        <v>9309</v>
+        <v>124221</v>
       </c>
       <c r="AI4">
-        <v>11895</v>
+        <v>157682</v>
       </c>
     </row>
     <row r="5" spans="1:35">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>112</v>
+        <v>24710</v>
       </c>
       <c r="C5">
-        <v>80</v>
+        <v>27288</v>
       </c>
       <c r="D5">
-        <v>77</v>
+        <v>30718</v>
       </c>
       <c r="E5">
-        <v>100</v>
+        <v>31468</v>
       </c>
       <c r="F5">
-        <v>124</v>
+        <v>33339</v>
       </c>
       <c r="G5">
-        <v>117</v>
+        <v>32029</v>
       </c>
       <c r="H5">
-        <v>169</v>
+        <v>36225</v>
       </c>
       <c r="I5">
-        <v>185</v>
+        <v>35706</v>
       </c>
       <c r="J5">
-        <v>146</v>
+        <v>37123</v>
       </c>
       <c r="K5">
-        <v>238</v>
+        <v>42169</v>
       </c>
       <c r="L5">
-        <v>303</v>
+        <v>42299</v>
       </c>
       <c r="M5">
-        <v>313</v>
+        <v>42081</v>
       </c>
       <c r="N5">
-        <v>423</v>
+        <v>47234</v>
       </c>
       <c r="O5">
-        <v>336</v>
+        <v>46948</v>
       </c>
       <c r="P5">
-        <v>399</v>
+        <v>54630</v>
       </c>
       <c r="Q5">
-        <v>421</v>
+        <v>54132</v>
       </c>
       <c r="R5">
-        <v>747</v>
+        <v>56344</v>
       </c>
       <c r="S5">
-        <v>612</v>
+        <v>57247</v>
       </c>
       <c r="T5">
-        <v>609</v>
+        <v>59390</v>
       </c>
       <c r="U5">
-        <v>592</v>
+        <v>59881</v>
       </c>
       <c r="V5">
-        <v>616</v>
+        <v>63032</v>
       </c>
       <c r="W5">
-        <v>600</v>
+        <v>68212</v>
       </c>
       <c r="X5">
-        <v>625</v>
+        <v>69975</v>
       </c>
       <c r="Y5">
-        <v>717</v>
+        <v>70520</v>
       </c>
       <c r="Z5">
-        <v>925</v>
+        <v>80083</v>
       </c>
       <c r="AA5">
-        <v>826</v>
+        <v>89816</v>
       </c>
       <c r="AB5">
-        <v>1065</v>
+        <v>101852</v>
       </c>
       <c r="AC5">
-        <v>1063</v>
+        <v>104463</v>
       </c>
       <c r="AD5">
-        <v>1285</v>
+        <v>108099</v>
       </c>
       <c r="AE5">
-        <v>1323</v>
+        <v>107482</v>
       </c>
       <c r="AF5">
-        <v>1285</v>
+        <v>110806</v>
       </c>
       <c r="AG5">
-        <v>1568</v>
+        <v>125817</v>
       </c>
       <c r="AH5">
-        <v>1755</v>
+        <v>143704</v>
       </c>
       <c r="AI5">
-        <v>2495</v>
+        <v>186834</v>
       </c>
     </row>
     <row r="6" spans="1:35">
       <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1232</v>
+      </c>
+      <c r="C6">
+        <v>1221</v>
+      </c>
+      <c r="D6">
+        <v>1400</v>
+      </c>
+      <c r="E6">
+        <v>1508</v>
+      </c>
+      <c r="F6">
+        <v>1670</v>
+      </c>
+      <c r="G6">
+        <v>1623</v>
+      </c>
+      <c r="H6">
+        <v>2012</v>
+      </c>
+      <c r="I6">
+        <v>2088</v>
+      </c>
+      <c r="J6">
+        <v>2204</v>
+      </c>
+      <c r="K6">
+        <v>2190</v>
+      </c>
+      <c r="L6">
+        <v>2283</v>
+      </c>
+      <c r="M6">
+        <v>2528</v>
+      </c>
+      <c r="N6">
+        <v>2903</v>
+      </c>
+      <c r="O6">
+        <v>2767</v>
+      </c>
+      <c r="P6">
+        <v>3586</v>
+      </c>
+      <c r="Q6">
+        <v>3283</v>
+      </c>
+      <c r="R6">
+        <v>3427</v>
+      </c>
+      <c r="S6">
+        <v>3331</v>
+      </c>
+      <c r="T6">
+        <v>3546</v>
+      </c>
+      <c r="U6">
+        <v>3762</v>
+      </c>
+      <c r="V6">
+        <v>4118</v>
+      </c>
+      <c r="W6">
+        <v>4417</v>
+      </c>
+      <c r="X6">
+        <v>4418</v>
+      </c>
+      <c r="Y6">
+        <v>4547</v>
+      </c>
+      <c r="Z6">
+        <v>5044</v>
+      </c>
+      <c r="AA6">
+        <v>5077</v>
+      </c>
+      <c r="AB6">
+        <v>6222</v>
+      </c>
+      <c r="AC6">
+        <v>6233</v>
+      </c>
+      <c r="AD6">
+        <v>6377</v>
+      </c>
+      <c r="AE6">
+        <v>6354</v>
+      </c>
+      <c r="AF6">
+        <v>6692</v>
+      </c>
+      <c r="AG6">
+        <v>8076</v>
+      </c>
+      <c r="AH6">
+        <v>9309</v>
+      </c>
+      <c r="AI6">
+        <v>11895</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>112</v>
+      </c>
+      <c r="C7">
+        <v>80</v>
+      </c>
+      <c r="D7">
+        <v>77</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>124</v>
+      </c>
+      <c r="G7">
+        <v>117</v>
+      </c>
+      <c r="H7">
+        <v>169</v>
+      </c>
+      <c r="I7">
+        <v>185</v>
+      </c>
+      <c r="J7">
+        <v>146</v>
+      </c>
+      <c r="K7">
+        <v>238</v>
+      </c>
+      <c r="L7">
+        <v>303</v>
+      </c>
+      <c r="M7">
+        <v>313</v>
+      </c>
+      <c r="N7">
+        <v>423</v>
+      </c>
+      <c r="O7">
+        <v>336</v>
+      </c>
+      <c r="P7">
+        <v>399</v>
+      </c>
+      <c r="Q7">
+        <v>421</v>
+      </c>
+      <c r="R7">
+        <v>747</v>
+      </c>
+      <c r="S7">
+        <v>612</v>
+      </c>
+      <c r="T7">
+        <v>609</v>
+      </c>
+      <c r="U7">
+        <v>592</v>
+      </c>
+      <c r="V7">
+        <v>616</v>
+      </c>
+      <c r="W7">
+        <v>600</v>
+      </c>
+      <c r="X7">
+        <v>625</v>
+      </c>
+      <c r="Y7">
+        <v>717</v>
+      </c>
+      <c r="Z7">
+        <v>925</v>
+      </c>
+      <c r="AA7">
+        <v>826</v>
+      </c>
+      <c r="AB7">
+        <v>1065</v>
+      </c>
+      <c r="AC7">
+        <v>1063</v>
+      </c>
+      <c r="AD7">
+        <v>1285</v>
+      </c>
+      <c r="AE7">
+        <v>1323</v>
+      </c>
+      <c r="AF7">
+        <v>1285</v>
+      </c>
+      <c r="AG7">
+        <v>1568</v>
+      </c>
+      <c r="AH7">
+        <v>1755</v>
+      </c>
+      <c r="AI7">
+        <v>2495</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B8">
         <v>0</v>
       </c>
-      <c r="C6">
+      <c r="C8">
         <v>0</v>
       </c>
-      <c r="D6">
+      <c r="D8">
         <v>0</v>
       </c>
-      <c r="E6">
+      <c r="E8">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="F8">
         <v>0</v>
       </c>
-      <c r="G6">
+      <c r="G8">
         <v>1005</v>
       </c>
-      <c r="H6">
+      <c r="H8">
         <v>942</v>
       </c>
-      <c r="I6">
+      <c r="I8">
         <v>1077</v>
       </c>
-      <c r="J6">
+      <c r="J8">
         <v>2343</v>
       </c>
-      <c r="K6">
+      <c r="K8">
         <v>2777</v>
       </c>
-      <c r="L6">
+      <c r="L8">
         <v>2512</v>
       </c>
-      <c r="M6">
+      <c r="M8">
         <v>2344</v>
       </c>
-      <c r="N6">
+      <c r="N8">
         <v>2864</v>
       </c>
-      <c r="O6">
+      <c r="O8">
         <v>3079</v>
       </c>
-      <c r="P6">
+      <c r="P8">
         <v>3699</v>
       </c>
-      <c r="Q6">
+      <c r="Q8">
         <v>4242</v>
       </c>
-      <c r="R6">
+      <c r="R8">
         <v>4252</v>
       </c>
-      <c r="S6">
+      <c r="S8">
         <v>4542</v>
       </c>
-      <c r="T6">
+      <c r="T8">
         <v>4362</v>
       </c>
-      <c r="U6">
+      <c r="U8">
         <v>4376</v>
       </c>
-      <c r="V6">
+      <c r="V8">
         <v>5256</v>
       </c>
-      <c r="W6">
+      <c r="W8">
         <v>6511</v>
       </c>
-      <c r="X6">
+      <c r="X8">
         <v>6753</v>
       </c>
-      <c r="Y6">
+      <c r="Y8">
         <v>7366</v>
       </c>
-      <c r="Z6">
+      <c r="Z8">
         <v>8377</v>
       </c>
-      <c r="AA6">
+      <c r="AA8">
         <v>9948</v>
       </c>
-      <c r="AB6">
+      <c r="AB8">
         <v>10328</v>
       </c>
-      <c r="AC6">
+      <c r="AC8">
         <v>9846</v>
       </c>
-      <c r="AD6">
+      <c r="AD8">
         <v>10042</v>
       </c>
-      <c r="AE6">
+      <c r="AE8">
         <v>10403</v>
       </c>
-      <c r="AF6">
+      <c r="AF8">
         <v>10474</v>
       </c>
-      <c r="AG6">
+      <c r="AG8">
         <v>10832</v>
       </c>
-      <c r="AH6">
+      <c r="AH8">
         <v>13832</v>
       </c>
-      <c r="AI6">
+      <c r="AI8">
         <v>17213</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add missing languages. Implements #3
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -10,11 +10,14 @@
     <sheet name="stats.xlsx.csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_2014" localSheetId="0">stats.xlsx.csv!#REF!</definedName>
     <definedName name="_2014__1" localSheetId="0">stats.xlsx.csv!#REF!</definedName>
-    <definedName name="_2015" localSheetId="0">stats.xlsx.csv!$N$2:$Y$8</definedName>
+    <definedName name="_2014_1" localSheetId="0">stats.xlsx.csv!$Y$23:$Y$29</definedName>
+    <definedName name="_2015" localSheetId="0">stats.xlsx.csv!$N$3:$Y$15</definedName>
     <definedName name="_2015__1" localSheetId="0">stats.xlsx.csv!#REF!</definedName>
-    <definedName name="_2016" localSheetId="0">stats.xlsx.csv!$Z$2:$AI$8</definedName>
+    <definedName name="_2016" localSheetId="0">stats.xlsx.csv!$Z$3:$AI$15</definedName>
     <definedName name="_2016__1" localSheetId="0">stats.xlsx.csv!#REF!</definedName>
+    <definedName name="_2016_1" localSheetId="0">stats.xlsx.csv!#REF!</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -46,8 +49,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="2015.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="Macintosh HD:Users:ekeller:Downloads:2015.csv" decimal="," thousands=" ">
+  <connection id="2" name="2014.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:ekeller:Downloads:2014.csv" decimal="," thousands=" ">
       <textFields count="13">
         <textField/>
         <textField/>
@@ -65,7 +68,83 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="2016.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="3" name="2014.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:ekeller:go-workspace:src:github.com:emmanuel-keller:github-language-statistics:2014.csv" decimal="," thousands=" ">
+      <textFields count="13">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="2015 (1).csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:ekeller:Downloads:2015 (1).csv" decimal="," thousands=" ">
+      <textFields count="13">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="2015.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:ekeller:Downloads:2015.csv" decimal="," thousands=" ">
+      <textFields count="13">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="6" name="2016.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:ekeller:Downloads:2016.csv" decimal="," thousands=" ">
+      <textFields count="13">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="7" name="2016.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:ekeller:Downloads:2016.csv" decimal="," thousands=" ">
       <textFields count="13">
         <textField/>
@@ -88,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>C++</t>
   </si>
@@ -105,10 +184,31 @@
     <t>Swift</t>
   </si>
   <si>
-    <t>c#</t>
+    <t>Javascript</t>
   </si>
   <si>
-    <t>Javascript</t>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>Scala</t>
+  </si>
+  <si>
+    <t>PHP</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Perl</t>
+  </si>
+  <si>
+    <t>Objective C</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Ruby</t>
   </si>
 </sst>
 </file>
@@ -160,8 +260,70 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -183,7 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="79">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -192,6 +354,37 @@
     <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -200,6 +393,37 @@
     <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -236,7 +460,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C++</c:v>
+                  <c:v>C</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -362,106 +586,106 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>6503.0</c:v>
+                  <c:v>5973.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6411.0</c:v>
+                  <c:v>5983.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7917.0</c:v>
+                  <c:v>7551.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8154.0</c:v>
+                  <c:v>7288.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8562.0</c:v>
+                  <c:v>7579.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8072.0</c:v>
+                  <c:v>6904.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7925.0</c:v>
+                  <c:v>6681.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8163.0</c:v>
+                  <c:v>6375.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8836.0</c:v>
+                  <c:v>7574.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10216.0</c:v>
+                  <c:v>9754.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10868.0</c:v>
+                  <c:v>9254.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11422.0</c:v>
+                  <c:v>9340.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11397.0</c:v>
+                  <c:v>9260.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10929.0</c:v>
+                  <c:v>9064.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19709.0</c:v>
+                  <c:v>15241.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>17684.0</c:v>
+                  <c:v>14795.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17667.0</c:v>
+                  <c:v>13560.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15829.0</c:v>
+                  <c:v>12591.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14431.0</c:v>
+                  <c:v>11538.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>14771.0</c:v>
+                  <c:v>12067.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>15716.0</c:v>
+                  <c:v>12210.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>17459.0</c:v>
+                  <c:v>14105.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>18162.0</c:v>
+                  <c:v>15653.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>19497.0</c:v>
+                  <c:v>16198.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>19457.0</c:v>
+                  <c:v>15569.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>20193.0</c:v>
+                  <c:v>16988.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26515.0</c:v>
+                  <c:v>19904.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>26144.0</c:v>
+                  <c:v>19770.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>26067.0</c:v>
+                  <c:v>19405.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>24053.0</c:v>
+                  <c:v>18456.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>21107.0</c:v>
+                  <c:v>16719.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>23883.0</c:v>
+                  <c:v>18332.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>29582.0</c:v>
+                  <c:v>22438.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>42153.0</c:v>
+                  <c:v>31058.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -477,7 +701,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>c#</c:v>
+                  <c:v>C++</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -603,106 +827,106 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>4771.0</c:v>
+                  <c:v>6503.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4713.0</c:v>
+                  <c:v>6411.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5680.0</c:v>
+                  <c:v>7917.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5926.0</c:v>
+                  <c:v>8154.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6696.0</c:v>
+                  <c:v>8562.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6445.0</c:v>
+                  <c:v>8072.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6567.0</c:v>
+                  <c:v>7925.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6633.0</c:v>
+                  <c:v>8163.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7795.0</c:v>
+                  <c:v>8836.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8916.0</c:v>
+                  <c:v>10216.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9217.0</c:v>
+                  <c:v>10868.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9576.0</c:v>
+                  <c:v>11422.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10627.0</c:v>
+                  <c:v>11397.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10058.0</c:v>
+                  <c:v>10929.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17199.0</c:v>
+                  <c:v>19709.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15441.0</c:v>
+                  <c:v>17684.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16112.0</c:v>
+                  <c:v>17667.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14822.0</c:v>
+                  <c:v>15829.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14257.0</c:v>
+                  <c:v>14431.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>14418.0</c:v>
+                  <c:v>14771.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>15281.0</c:v>
+                  <c:v>15716.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>17759.0</c:v>
+                  <c:v>17459.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>18313.0</c:v>
+                  <c:v>18162.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>18731.0</c:v>
+                  <c:v>19497.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>19708.0</c:v>
+                  <c:v>19457.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>20986.0</c:v>
+                  <c:v>20193.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>23545.0</c:v>
+                  <c:v>26515.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>25404.0</c:v>
+                  <c:v>26144.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>25997.0</c:v>
+                  <c:v>26067.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>25417.0</c:v>
+                  <c:v>24053.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>23844.0</c:v>
+                  <c:v>21107.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>25884.0</c:v>
+                  <c:v>23883.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>30700.0</c:v>
+                  <c:v>29582.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>40536.0</c:v>
+                  <c:v>42153.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -718,7 +942,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Java</c:v>
+                  <c:v>C#</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -844,106 +1068,106 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>20766.0</c:v>
+                  <c:v>4771.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21414.0</c:v>
+                  <c:v>4713.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26178.0</c:v>
+                  <c:v>5680.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26748.0</c:v>
+                  <c:v>5926.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29169.0</c:v>
+                  <c:v>6696.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26278.0</c:v>
+                  <c:v>6445.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26420.0</c:v>
+                  <c:v>6567.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26041.0</c:v>
+                  <c:v>6633.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31238.0</c:v>
+                  <c:v>7795.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36233.0</c:v>
+                  <c:v>8916.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>38825.0</c:v>
+                  <c:v>9217.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>38814.0</c:v>
+                  <c:v>9576.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>40639.0</c:v>
+                  <c:v>10627.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>39273.0</c:v>
+                  <c:v>10058.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>66473.0</c:v>
+                  <c:v>17199.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>61641.0</c:v>
+                  <c:v>15441.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>62018.0</c:v>
+                  <c:v>16112.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>58580.0</c:v>
+                  <c:v>14822.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>54329.0</c:v>
+                  <c:v>14257.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>54980.0</c:v>
+                  <c:v>14418.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>61126.0</c:v>
+                  <c:v>15281.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>69324.0</c:v>
+                  <c:v>17759.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>72593.0</c:v>
+                  <c:v>18313.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>71850.0</c:v>
+                  <c:v>18731.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>72445.0</c:v>
+                  <c:v>19708.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>80629.0</c:v>
+                  <c:v>20986.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>103005.0</c:v>
+                  <c:v>23545.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>104095.0</c:v>
+                  <c:v>25404.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>101442.0</c:v>
+                  <c:v>25997.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>96881.0</c:v>
+                  <c:v>25417.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>92797.0</c:v>
+                  <c:v>23844.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>102902.0</c:v>
+                  <c:v>25884.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>124221.0</c:v>
+                  <c:v>30700.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>157682.0</c:v>
+                  <c:v>40536.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -959,6 +1183,257 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
+                  <c:v>Java</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="33"/>
+            <c:marker/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$1:$AI$1</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>40178.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40209.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40237.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40268.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40298.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40329.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40359.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40390.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40421.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40451.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40482.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40512.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40543.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40574.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40602.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40633.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40663.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40694.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40755.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40786.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40816.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40847.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40877.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40908.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40939.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40968.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40999.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41029.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41060.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41090.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41121.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41152.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41182.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$5:$AI$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>20766.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21414.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26178.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26748.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29169.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26278.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26420.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26041.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31238.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>36233.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>38825.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>38814.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40639.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39273.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>66473.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>61641.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>62018.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>58580.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>54329.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>54980.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>61126.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>69324.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>72593.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>71850.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>72445.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>80629.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>103005.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>104095.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>101442.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>96881.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>92797.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>102902.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>124221.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>157682.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stats.xlsx.csv!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
                   <c:v>Javascript</c:v>
                 </c:pt>
               </c:strCache>
@@ -1080,7 +1555,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats.xlsx.csv!$B$5:$AI$5</c:f>
+              <c:f>stats.xlsx.csv!$B$6:$AI$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1192,11 +1667,11 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
+          <c:idx val="5"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>stats.xlsx.csv!$A$6</c:f>
+              <c:f>stats.xlsx.csv!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1321,7 +1796,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats.xlsx.csv!$B$6:$AI$6</c:f>
+              <c:f>stats.xlsx.csv!$B$7:$AI$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1430,18 +1905,18 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
+          <c:idx val="6"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>stats.xlsx.csv!$A$7</c:f>
+              <c:f>stats.xlsx.csv!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rust</c:v>
+                  <c:v>Objective C</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1562,111 +2037,111 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats.xlsx.csv!$B$7:$AI$7</c:f>
+              <c:f>stats.xlsx.csv!$B$8:$AI$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>112.0</c:v>
+                  <c:v>32597.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80.0</c:v>
+                  <c:v>33831.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>77.0</c:v>
+                  <c:v>39377.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>41366.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>124.0</c:v>
+                  <c:v>42976.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>117.0</c:v>
+                  <c:v>40698.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>169.0</c:v>
+                  <c:v>45318.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>185.0</c:v>
+                  <c:v>47639.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>146.0</c:v>
+                  <c:v>46165.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>238.0</c:v>
+                  <c:v>59611.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>303.0</c:v>
+                  <c:v>52232.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>313.0</c:v>
+                  <c:v>52078.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>423.0</c:v>
+                  <c:v>65001.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>336.0</c:v>
+                  <c:v>59259.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>399.0</c:v>
+                  <c:v>80667.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>421.0</c:v>
+                  <c:v>77413.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>747.0</c:v>
+                  <c:v>77359.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>612.0</c:v>
+                  <c:v>73474.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>609.0</c:v>
+                  <c:v>74640.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>592.0</c:v>
+                  <c:v>81358.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>616.0</c:v>
+                  <c:v>82691.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>600.0</c:v>
+                  <c:v>90888.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>625.0</c:v>
+                  <c:v>92348.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>717.0</c:v>
+                  <c:v>95260.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>925.0</c:v>
+                  <c:v>101205.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>826.0</c:v>
+                  <c:v>115529.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1065.0</c:v>
+                  <c:v>130352.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1063.0</c:v>
+                  <c:v>135694.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1285.0</c:v>
+                  <c:v>139299.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1323.0</c:v>
+                  <c:v>134540.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1285.0</c:v>
+                  <c:v>139650.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1568.0</c:v>
+                  <c:v>151842.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1755.0</c:v>
+                  <c:v>179472.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2495.0</c:v>
+                  <c:v>224544.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1674,15 +2149,15 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
+          <c:idx val="7"/>
+          <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>stats.xlsx.csv!$A$8</c:f>
+              <c:f>stats.xlsx.csv!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Swift</c:v>
+                  <c:v>Perl</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1803,7 +2278,1453 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats.xlsx.csv!$B$8:$AI$8</c:f>
+              <c:f>stats.xlsx.csv!$B$9:$AI$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>1051.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>992.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1052.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1082.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1092.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1107.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1180.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1404.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1428.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32410.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2758.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1268.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3234.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1250.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1798.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1377.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1769.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1317.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1312.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1470.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1505.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1560.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1662.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1485.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1630.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1785.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2505.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1978.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1905.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2070.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1941.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2241.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2709.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3773.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stats.xlsx.csv!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PHP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$1:$AI$1</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>40178.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40209.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40237.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40268.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40298.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40329.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40359.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40390.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40421.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40451.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40482.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40512.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40543.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40574.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40602.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40633.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40663.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40694.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40755.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40786.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40816.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40847.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40877.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40908.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40939.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40968.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40999.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41029.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41060.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41090.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41121.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41152.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41182.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$10:$AI$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>11041.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10753.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12185.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12061.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12517.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12272.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13543.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13471.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14260.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16262.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16210.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16201.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17435.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17900.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24292.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>22901.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22785.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22526.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22443.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23663.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>22031.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>24167.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>25890.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24594.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26585.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>29591.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>33234.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>33300.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>34783.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>35181.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>34351.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>39336.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>45122.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>58247.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stats.xlsx.csv!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Python</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$1:$AI$1</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>40178.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40209.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40237.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40268.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40298.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40329.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40359.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40390.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40421.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40451.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40482.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40512.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40543.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40574.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40602.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40633.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40663.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40694.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40755.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40786.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40816.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40847.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40877.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40908.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40939.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40968.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40999.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41029.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41060.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41090.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41121.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41152.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41182.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$11:$AI$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>11795.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12451.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14713.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14337.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15079.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14529.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15655.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15711.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16412.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20484.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19342.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20044.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21413.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20890.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29747.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>27976.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27809.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27394.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>27244.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27826.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30118.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>33225.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>34299.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>35811.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>37972.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40306.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>47896.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>49210.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>49869.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>48832.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>50398.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>57055.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>66363.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>89880.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stats.xlsx.csv!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ruby</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$1:$AI$1</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>40178.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40209.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40237.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40268.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40298.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40329.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40359.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40390.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40421.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40451.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40482.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40512.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40543.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40574.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40602.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40633.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40663.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40694.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40755.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40786.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40816.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40847.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40877.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40908.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40939.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40968.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40999.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41029.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41060.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41090.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41121.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41152.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41182.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$12:$AI$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>15599.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16003.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18016.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17250.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17463.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16580.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19114.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18102.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17729.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18552.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17927.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16985.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18942.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20337.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21702.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21269.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20565.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21614.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22125.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21761.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>22640.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25408.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22124.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>20275.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22107.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>24712.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>25701.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>25611.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>26705.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>26032.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>26401.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>28882.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>31104.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>38338.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stats.xlsx.csv!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rust</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$1:$AI$1</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>40178.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40209.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40237.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40268.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40298.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40329.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40359.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40390.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40421.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40451.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40482.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40512.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40543.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40574.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40602.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40633.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40663.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40694.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40755.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40786.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40816.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40847.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40877.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40908.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40939.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40968.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40999.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41029.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41060.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41090.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41121.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41152.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41182.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$13:$AI$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>112.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>117.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>169.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>185.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>146.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>238.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>303.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>313.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>423.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>336.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>399.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>421.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>747.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>612.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>609.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>592.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>616.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>625.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>717.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>925.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>826.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1065.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1063.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1285.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1323.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1285.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1568.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1755.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2495.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stats.xlsx.csv!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Scala</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$1:$AI$1</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>40178.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40209.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40237.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40268.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40298.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40329.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40359.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40390.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40421.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40451.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40482.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40512.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40543.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40574.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40602.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40633.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40663.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40694.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40755.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40786.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40816.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40847.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40877.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40908.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40939.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40968.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40999.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41029.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41060.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41090.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41121.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41152.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41182.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$14:$AI$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>870.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>856.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>865.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>933.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1082.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1089.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1017.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>991.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1074.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1234.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1272.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1322.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1433.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1479.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1778.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1682.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1822.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1694.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1729.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1626.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1744.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1987.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1954.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2106.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2221.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2184.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2575.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2551.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2756.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2772.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2781.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3048.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3619.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4700.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stats.xlsx.csv!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Swift</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$1:$AI$1</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>40178.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40209.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40237.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40268.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40298.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40329.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40359.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40390.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40421.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40451.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40482.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40512.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40543.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40574.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40602.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40633.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40663.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40694.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40755.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40786.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40816.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40847.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40877.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40908.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40939.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40968.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40999.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41029.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41060.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41090.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41121.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41152.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41182.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$15:$AI$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1924,11 +3845,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2124205672"/>
-        <c:axId val="2124208856"/>
+        <c:axId val="2055851416"/>
+        <c:axId val="2056816264"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2124205672"/>
+        <c:axId val="2055851416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1948,14 +3869,14 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2124208856"/>
+        <c:crossAx val="2056816264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2124208856"/>
+        <c:axId val="2056816264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1977,7 +3898,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2124205672"/>
+        <c:crossAx val="2055851416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1988,10 +3909,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0582374737759856"/>
-          <c:y val="0.0132669983416252"/>
-          <c:w val="0.941762526224014"/>
-          <c:h val="0.0533429963045664"/>
+          <c:x val="0.164775540600677"/>
+          <c:y val="0.00379867046533713"/>
+          <c:w val="0.670448827979548"/>
+          <c:h val="0.0897411968803045"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -2023,15 +3944,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2054,11 +3975,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2016" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2014_1" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2015" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2015" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2016" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2383,15 +4308,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI8"/>
+  <dimension ref="A1:AI15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
@@ -2416,14 +4341,10 @@
     <col min="23" max="23" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="29" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.1640625" customWidth="1"/>
-    <col min="33" max="35" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="7.1640625" customWidth="1"/>
+    <col min="31" max="35" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="6.1640625" customWidth="1"/>
     <col min="38" max="38" width="2.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2533,750 +4454,1499 @@
     </row>
     <row r="2" spans="1:35">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B2">
-        <v>6503</v>
+        <v>5973</v>
       </c>
       <c r="C2">
-        <v>6411</v>
+        <v>5983</v>
       </c>
       <c r="D2">
-        <v>7917</v>
+        <v>7551</v>
       </c>
       <c r="E2">
-        <v>8154</v>
+        <v>7288</v>
       </c>
       <c r="F2">
-        <v>8562</v>
+        <v>7579</v>
       </c>
       <c r="G2">
-        <v>8072</v>
+        <v>6904</v>
       </c>
       <c r="H2">
-        <v>7925</v>
+        <v>6681</v>
       </c>
       <c r="I2">
-        <v>8163</v>
+        <v>6375</v>
       </c>
       <c r="J2">
-        <v>8836</v>
+        <v>7574</v>
       </c>
       <c r="K2">
-        <v>10216</v>
+        <v>9754</v>
       </c>
       <c r="L2">
-        <v>10868</v>
+        <v>9254</v>
       </c>
       <c r="M2">
-        <v>11422</v>
+        <v>9340</v>
       </c>
       <c r="N2">
-        <v>11397</v>
+        <v>9260</v>
       </c>
       <c r="O2">
-        <v>10929</v>
+        <v>9064</v>
       </c>
       <c r="P2">
-        <v>19709</v>
+        <v>15241</v>
       </c>
       <c r="Q2">
-        <v>17684</v>
+        <v>14795</v>
       </c>
       <c r="R2">
-        <v>17667</v>
+        <v>13560</v>
       </c>
       <c r="S2">
-        <v>15829</v>
+        <v>12591</v>
       </c>
       <c r="T2">
-        <v>14431</v>
+        <v>11538</v>
       </c>
       <c r="U2">
-        <v>14771</v>
+        <v>12067</v>
       </c>
       <c r="V2">
-        <v>15716</v>
+        <v>12210</v>
       </c>
       <c r="W2">
-        <v>17459</v>
+        <v>14105</v>
       </c>
       <c r="X2">
-        <v>18162</v>
+        <v>15653</v>
       </c>
       <c r="Y2">
-        <v>19497</v>
+        <v>16198</v>
       </c>
       <c r="Z2">
-        <v>19457</v>
+        <v>15569</v>
       </c>
       <c r="AA2">
-        <v>20193</v>
+        <v>16988</v>
       </c>
       <c r="AB2">
-        <v>26515</v>
+        <v>19904</v>
       </c>
       <c r="AC2">
-        <v>26144</v>
+        <v>19770</v>
       </c>
       <c r="AD2">
-        <v>26067</v>
+        <v>19405</v>
       </c>
       <c r="AE2">
-        <v>24053</v>
+        <v>18456</v>
       </c>
       <c r="AF2">
-        <v>21107</v>
+        <v>16719</v>
       </c>
       <c r="AG2">
-        <v>23883</v>
+        <v>18332</v>
       </c>
       <c r="AH2">
-        <v>29582</v>
+        <v>22438</v>
       </c>
       <c r="AI2">
-        <v>42153</v>
+        <v>31058</v>
       </c>
     </row>
     <row r="3" spans="1:35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>4771</v>
+        <v>6503</v>
       </c>
       <c r="C3">
-        <v>4713</v>
+        <v>6411</v>
       </c>
       <c r="D3">
-        <v>5680</v>
+        <v>7917</v>
       </c>
       <c r="E3">
-        <v>5926</v>
+        <v>8154</v>
       </c>
       <c r="F3">
-        <v>6696</v>
+        <v>8562</v>
       </c>
       <c r="G3">
-        <v>6445</v>
+        <v>8072</v>
       </c>
       <c r="H3">
-        <v>6567</v>
+        <v>7925</v>
       </c>
       <c r="I3">
-        <v>6633</v>
+        <v>8163</v>
       </c>
       <c r="J3">
-        <v>7795</v>
+        <v>8836</v>
       </c>
       <c r="K3">
-        <v>8916</v>
+        <v>10216</v>
       </c>
       <c r="L3">
-        <v>9217</v>
+        <v>10868</v>
       </c>
       <c r="M3">
-        <v>9576</v>
+        <v>11422</v>
       </c>
       <c r="N3">
-        <v>10627</v>
+        <v>11397</v>
       </c>
       <c r="O3">
-        <v>10058</v>
+        <v>10929</v>
       </c>
       <c r="P3">
-        <v>17199</v>
+        <v>19709</v>
       </c>
       <c r="Q3">
-        <v>15441</v>
+        <v>17684</v>
       </c>
       <c r="R3">
-        <v>16112</v>
+        <v>17667</v>
       </c>
       <c r="S3">
-        <v>14822</v>
+        <v>15829</v>
       </c>
       <c r="T3">
-        <v>14257</v>
+        <v>14431</v>
       </c>
       <c r="U3">
-        <v>14418</v>
+        <v>14771</v>
       </c>
       <c r="V3">
-        <v>15281</v>
+        <v>15716</v>
       </c>
       <c r="W3">
-        <v>17759</v>
+        <v>17459</v>
       </c>
       <c r="X3">
-        <v>18313</v>
+        <v>18162</v>
       </c>
       <c r="Y3">
-        <v>18731</v>
+        <v>19497</v>
       </c>
       <c r="Z3">
-        <v>19708</v>
+        <v>19457</v>
       </c>
       <c r="AA3">
-        <v>20986</v>
+        <v>20193</v>
       </c>
       <c r="AB3">
-        <v>23545</v>
+        <v>26515</v>
       </c>
       <c r="AC3">
-        <v>25404</v>
+        <v>26144</v>
       </c>
       <c r="AD3">
-        <v>25997</v>
+        <v>26067</v>
       </c>
       <c r="AE3">
-        <v>25417</v>
+        <v>24053</v>
       </c>
       <c r="AF3">
-        <v>23844</v>
+        <v>21107</v>
       </c>
       <c r="AG3">
-        <v>25884</v>
+        <v>23883</v>
       </c>
       <c r="AH3">
-        <v>30700</v>
+        <v>29582</v>
       </c>
       <c r="AI3">
-        <v>40536</v>
+        <v>42153</v>
       </c>
     </row>
     <row r="4" spans="1:35">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>20766</v>
+        <v>4771</v>
       </c>
       <c r="C4">
-        <v>21414</v>
+        <v>4713</v>
       </c>
       <c r="D4">
-        <v>26178</v>
+        <v>5680</v>
       </c>
       <c r="E4">
-        <v>26748</v>
+        <v>5926</v>
       </c>
       <c r="F4">
-        <v>29169</v>
+        <v>6696</v>
       </c>
       <c r="G4">
-        <v>26278</v>
+        <v>6445</v>
       </c>
       <c r="H4">
-        <v>26420</v>
+        <v>6567</v>
       </c>
       <c r="I4">
-        <v>26041</v>
+        <v>6633</v>
       </c>
       <c r="J4">
-        <v>31238</v>
+        <v>7795</v>
       </c>
       <c r="K4">
-        <v>36233</v>
+        <v>8916</v>
       </c>
       <c r="L4">
-        <v>38825</v>
+        <v>9217</v>
       </c>
       <c r="M4">
-        <v>38814</v>
+        <v>9576</v>
       </c>
       <c r="N4">
-        <v>40639</v>
+        <v>10627</v>
       </c>
       <c r="O4">
-        <v>39273</v>
+        <v>10058</v>
       </c>
       <c r="P4">
-        <v>66473</v>
+        <v>17199</v>
       </c>
       <c r="Q4">
-        <v>61641</v>
+        <v>15441</v>
       </c>
       <c r="R4">
-        <v>62018</v>
+        <v>16112</v>
       </c>
       <c r="S4">
-        <v>58580</v>
+        <v>14822</v>
       </c>
       <c r="T4">
-        <v>54329</v>
+        <v>14257</v>
       </c>
       <c r="U4">
-        <v>54980</v>
+        <v>14418</v>
       </c>
       <c r="V4">
-        <v>61126</v>
+        <v>15281</v>
       </c>
       <c r="W4">
-        <v>69324</v>
+        <v>17759</v>
       </c>
       <c r="X4">
-        <v>72593</v>
+        <v>18313</v>
       </c>
       <c r="Y4">
-        <v>71850</v>
+        <v>18731</v>
       </c>
       <c r="Z4">
-        <v>72445</v>
+        <v>19708</v>
       </c>
       <c r="AA4">
-        <v>80629</v>
+        <v>20986</v>
       </c>
       <c r="AB4">
-        <v>103005</v>
+        <v>23545</v>
       </c>
       <c r="AC4">
-        <v>104095</v>
+        <v>25404</v>
       </c>
       <c r="AD4">
-        <v>101442</v>
+        <v>25997</v>
       </c>
       <c r="AE4">
-        <v>96881</v>
+        <v>25417</v>
       </c>
       <c r="AF4">
-        <v>92797</v>
+        <v>23844</v>
       </c>
       <c r="AG4">
-        <v>102902</v>
+        <v>25884</v>
       </c>
       <c r="AH4">
-        <v>124221</v>
+        <v>30700</v>
       </c>
       <c r="AI4">
-        <v>157682</v>
+        <v>40536</v>
       </c>
     </row>
     <row r="5" spans="1:35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>24710</v>
+        <v>20766</v>
       </c>
       <c r="C5">
-        <v>27288</v>
+        <v>21414</v>
       </c>
       <c r="D5">
-        <v>30718</v>
+        <v>26178</v>
       </c>
       <c r="E5">
-        <v>31468</v>
+        <v>26748</v>
       </c>
       <c r="F5">
-        <v>33339</v>
+        <v>29169</v>
       </c>
       <c r="G5">
-        <v>32029</v>
+        <v>26278</v>
       </c>
       <c r="H5">
-        <v>36225</v>
+        <v>26420</v>
       </c>
       <c r="I5">
-        <v>35706</v>
+        <v>26041</v>
       </c>
       <c r="J5">
-        <v>37123</v>
+        <v>31238</v>
       </c>
       <c r="K5">
-        <v>42169</v>
+        <v>36233</v>
       </c>
       <c r="L5">
-        <v>42299</v>
+        <v>38825</v>
       </c>
       <c r="M5">
-        <v>42081</v>
+        <v>38814</v>
       </c>
       <c r="N5">
-        <v>47234</v>
+        <v>40639</v>
       </c>
       <c r="O5">
-        <v>46948</v>
+        <v>39273</v>
       </c>
       <c r="P5">
-        <v>54630</v>
+        <v>66473</v>
       </c>
       <c r="Q5">
-        <v>54132</v>
+        <v>61641</v>
       </c>
       <c r="R5">
-        <v>56344</v>
+        <v>62018</v>
       </c>
       <c r="S5">
-        <v>57247</v>
+        <v>58580</v>
       </c>
       <c r="T5">
-        <v>59390</v>
+        <v>54329</v>
       </c>
       <c r="U5">
-        <v>59881</v>
+        <v>54980</v>
       </c>
       <c r="V5">
-        <v>63032</v>
+        <v>61126</v>
       </c>
       <c r="W5">
-        <v>68212</v>
+        <v>69324</v>
       </c>
       <c r="X5">
-        <v>69975</v>
+        <v>72593</v>
       </c>
       <c r="Y5">
-        <v>70520</v>
+        <v>71850</v>
       </c>
       <c r="Z5">
-        <v>80083</v>
+        <v>72445</v>
       </c>
       <c r="AA5">
-        <v>89816</v>
+        <v>80629</v>
       </c>
       <c r="AB5">
-        <v>101852</v>
+        <v>103005</v>
       </c>
       <c r="AC5">
-        <v>104463</v>
+        <v>104095</v>
       </c>
       <c r="AD5">
-        <v>108099</v>
+        <v>101442</v>
       </c>
       <c r="AE5">
-        <v>107482</v>
+        <v>96881</v>
       </c>
       <c r="AF5">
-        <v>110806</v>
+        <v>92797</v>
       </c>
       <c r="AG5">
-        <v>125817</v>
+        <v>102902</v>
       </c>
       <c r="AH5">
-        <v>143704</v>
+        <v>124221</v>
       </c>
       <c r="AI5">
-        <v>186834</v>
+        <v>157682</v>
       </c>
     </row>
     <row r="6" spans="1:35">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>1232</v>
+        <v>24710</v>
       </c>
       <c r="C6">
-        <v>1221</v>
+        <v>27288</v>
       </c>
       <c r="D6">
-        <v>1400</v>
+        <v>30718</v>
       </c>
       <c r="E6">
-        <v>1508</v>
+        <v>31468</v>
       </c>
       <c r="F6">
-        <v>1670</v>
+        <v>33339</v>
       </c>
       <c r="G6">
-        <v>1623</v>
+        <v>32029</v>
       </c>
       <c r="H6">
-        <v>2012</v>
+        <v>36225</v>
       </c>
       <c r="I6">
-        <v>2088</v>
+        <v>35706</v>
       </c>
       <c r="J6">
-        <v>2204</v>
+        <v>37123</v>
       </c>
       <c r="K6">
-        <v>2190</v>
+        <v>42169</v>
       </c>
       <c r="L6">
-        <v>2283</v>
+        <v>42299</v>
       </c>
       <c r="M6">
-        <v>2528</v>
+        <v>42081</v>
       </c>
       <c r="N6">
-        <v>2903</v>
+        <v>47234</v>
       </c>
       <c r="O6">
-        <v>2767</v>
+        <v>46948</v>
       </c>
       <c r="P6">
-        <v>3586</v>
+        <v>54630</v>
       </c>
       <c r="Q6">
-        <v>3283</v>
+        <v>54132</v>
       </c>
       <c r="R6">
-        <v>3427</v>
+        <v>56344</v>
       </c>
       <c r="S6">
-        <v>3331</v>
+        <v>57247</v>
       </c>
       <c r="T6">
-        <v>3546</v>
+        <v>59390</v>
       </c>
       <c r="U6">
-        <v>3762</v>
+        <v>59881</v>
       </c>
       <c r="V6">
-        <v>4118</v>
+        <v>63032</v>
       </c>
       <c r="W6">
-        <v>4417</v>
+        <v>68212</v>
       </c>
       <c r="X6">
-        <v>4418</v>
+        <v>69975</v>
       </c>
       <c r="Y6">
-        <v>4547</v>
+        <v>70520</v>
       </c>
       <c r="Z6">
-        <v>5044</v>
+        <v>80083</v>
       </c>
       <c r="AA6">
-        <v>5077</v>
+        <v>89816</v>
       </c>
       <c r="AB6">
-        <v>6222</v>
+        <v>101852</v>
       </c>
       <c r="AC6">
-        <v>6233</v>
+        <v>104463</v>
       </c>
       <c r="AD6">
-        <v>6377</v>
+        <v>108099</v>
       </c>
       <c r="AE6">
-        <v>6354</v>
+        <v>107482</v>
       </c>
       <c r="AF6">
-        <v>6692</v>
+        <v>110806</v>
       </c>
       <c r="AG6">
-        <v>8076</v>
+        <v>125817</v>
       </c>
       <c r="AH6">
-        <v>9309</v>
+        <v>143704</v>
       </c>
       <c r="AI6">
-        <v>11895</v>
+        <v>186834</v>
       </c>
     </row>
     <row r="7" spans="1:35">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>112</v>
+        <v>1232</v>
       </c>
       <c r="C7">
-        <v>80</v>
+        <v>1221</v>
       </c>
       <c r="D7">
-        <v>77</v>
+        <v>1400</v>
       </c>
       <c r="E7">
-        <v>100</v>
+        <v>1508</v>
       </c>
       <c r="F7">
-        <v>124</v>
+        <v>1670</v>
       </c>
       <c r="G7">
-        <v>117</v>
+        <v>1623</v>
       </c>
       <c r="H7">
-        <v>169</v>
+        <v>2012</v>
       </c>
       <c r="I7">
-        <v>185</v>
+        <v>2088</v>
       </c>
       <c r="J7">
-        <v>146</v>
+        <v>2204</v>
       </c>
       <c r="K7">
-        <v>238</v>
+        <v>2190</v>
       </c>
       <c r="L7">
-        <v>303</v>
+        <v>2283</v>
       </c>
       <c r="M7">
-        <v>313</v>
+        <v>2528</v>
       </c>
       <c r="N7">
-        <v>423</v>
+        <v>2903</v>
       </c>
       <c r="O7">
-        <v>336</v>
+        <v>2767</v>
       </c>
       <c r="P7">
-        <v>399</v>
+        <v>3586</v>
       </c>
       <c r="Q7">
-        <v>421</v>
+        <v>3283</v>
       </c>
       <c r="R7">
-        <v>747</v>
+        <v>3427</v>
       </c>
       <c r="S7">
-        <v>612</v>
+        <v>3331</v>
       </c>
       <c r="T7">
-        <v>609</v>
+        <v>3546</v>
       </c>
       <c r="U7">
-        <v>592</v>
+        <v>3762</v>
       </c>
       <c r="V7">
-        <v>616</v>
+        <v>4118</v>
       </c>
       <c r="W7">
-        <v>600</v>
+        <v>4417</v>
       </c>
       <c r="X7">
-        <v>625</v>
+        <v>4418</v>
       </c>
       <c r="Y7">
-        <v>717</v>
+        <v>4547</v>
       </c>
       <c r="Z7">
-        <v>925</v>
+        <v>5044</v>
       </c>
       <c r="AA7">
-        <v>826</v>
+        <v>5077</v>
       </c>
       <c r="AB7">
-        <v>1065</v>
+        <v>6222</v>
       </c>
       <c r="AC7">
-        <v>1063</v>
+        <v>6233</v>
       </c>
       <c r="AD7">
-        <v>1285</v>
+        <v>6377</v>
       </c>
       <c r="AE7">
-        <v>1323</v>
+        <v>6354</v>
       </c>
       <c r="AF7">
-        <v>1285</v>
+        <v>6692</v>
       </c>
       <c r="AG7">
-        <v>1568</v>
+        <v>8076</v>
       </c>
       <c r="AH7">
-        <v>1755</v>
+        <v>9309</v>
       </c>
       <c r="AI7">
-        <v>2495</v>
+        <v>11895</v>
       </c>
     </row>
     <row r="8" spans="1:35">
       <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>32597</v>
+      </c>
+      <c r="C8">
+        <v>33831</v>
+      </c>
+      <c r="D8">
+        <v>39377</v>
+      </c>
+      <c r="E8">
+        <v>41366</v>
+      </c>
+      <c r="F8">
+        <v>42976</v>
+      </c>
+      <c r="G8">
+        <v>40698</v>
+      </c>
+      <c r="H8">
+        <v>45318</v>
+      </c>
+      <c r="I8">
+        <v>47639</v>
+      </c>
+      <c r="J8">
+        <v>46165</v>
+      </c>
+      <c r="K8">
+        <v>59611</v>
+      </c>
+      <c r="L8">
+        <v>52232</v>
+      </c>
+      <c r="M8">
+        <v>52078</v>
+      </c>
+      <c r="N8">
+        <v>65001</v>
+      </c>
+      <c r="O8">
+        <v>59259</v>
+      </c>
+      <c r="P8">
+        <v>80667</v>
+      </c>
+      <c r="Q8">
+        <v>77413</v>
+      </c>
+      <c r="R8">
+        <v>77359</v>
+      </c>
+      <c r="S8">
+        <v>73474</v>
+      </c>
+      <c r="T8">
+        <v>74640</v>
+      </c>
+      <c r="U8">
+        <v>81358</v>
+      </c>
+      <c r="V8">
+        <v>82691</v>
+      </c>
+      <c r="W8">
+        <v>90888</v>
+      </c>
+      <c r="X8">
+        <v>92348</v>
+      </c>
+      <c r="Y8">
+        <v>95260</v>
+      </c>
+      <c r="Z8">
+        <v>101205</v>
+      </c>
+      <c r="AA8">
+        <v>115529</v>
+      </c>
+      <c r="AB8">
+        <v>130352</v>
+      </c>
+      <c r="AC8">
+        <v>135694</v>
+      </c>
+      <c r="AD8">
+        <v>139299</v>
+      </c>
+      <c r="AE8">
+        <v>134540</v>
+      </c>
+      <c r="AF8">
+        <v>139650</v>
+      </c>
+      <c r="AG8">
+        <v>151842</v>
+      </c>
+      <c r="AH8">
+        <v>179472</v>
+      </c>
+      <c r="AI8">
+        <v>224544</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>1051</v>
+      </c>
+      <c r="C9">
+        <v>992</v>
+      </c>
+      <c r="D9">
+        <v>1052</v>
+      </c>
+      <c r="E9">
+        <v>1082</v>
+      </c>
+      <c r="F9">
+        <v>1092</v>
+      </c>
+      <c r="G9">
+        <v>1107</v>
+      </c>
+      <c r="H9">
+        <v>1180</v>
+      </c>
+      <c r="I9">
+        <v>1404</v>
+      </c>
+      <c r="J9">
+        <v>1428</v>
+      </c>
+      <c r="K9">
+        <v>32410</v>
+      </c>
+      <c r="L9">
+        <v>2758</v>
+      </c>
+      <c r="M9">
+        <v>1268</v>
+      </c>
+      <c r="N9">
+        <v>3234</v>
+      </c>
+      <c r="O9">
+        <v>1250</v>
+      </c>
+      <c r="P9">
+        <v>1798</v>
+      </c>
+      <c r="Q9">
+        <v>1377</v>
+      </c>
+      <c r="R9">
+        <v>1769</v>
+      </c>
+      <c r="S9">
+        <v>1317</v>
+      </c>
+      <c r="T9">
+        <v>1312</v>
+      </c>
+      <c r="U9">
+        <v>1470</v>
+      </c>
+      <c r="V9">
+        <v>1505</v>
+      </c>
+      <c r="W9">
+        <v>1560</v>
+      </c>
+      <c r="X9">
+        <v>1662</v>
+      </c>
+      <c r="Y9">
+        <v>1485</v>
+      </c>
+      <c r="Z9">
+        <v>1630</v>
+      </c>
+      <c r="AA9">
+        <v>1785</v>
+      </c>
+      <c r="AB9">
+        <v>2505</v>
+      </c>
+      <c r="AC9">
+        <v>1978</v>
+      </c>
+      <c r="AD9">
+        <v>1905</v>
+      </c>
+      <c r="AE9">
+        <v>2070</v>
+      </c>
+      <c r="AF9">
+        <v>1941</v>
+      </c>
+      <c r="AG9">
+        <v>2241</v>
+      </c>
+      <c r="AH9">
+        <v>2709</v>
+      </c>
+      <c r="AI9">
+        <v>3773</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>11041</v>
+      </c>
+      <c r="C10">
+        <v>10753</v>
+      </c>
+      <c r="D10">
+        <v>12185</v>
+      </c>
+      <c r="E10">
+        <v>12061</v>
+      </c>
+      <c r="F10">
+        <v>12517</v>
+      </c>
+      <c r="G10">
+        <v>12272</v>
+      </c>
+      <c r="H10">
+        <v>13543</v>
+      </c>
+      <c r="I10">
+        <v>13471</v>
+      </c>
+      <c r="J10">
+        <v>14260</v>
+      </c>
+      <c r="K10">
+        <v>16262</v>
+      </c>
+      <c r="L10">
+        <v>16210</v>
+      </c>
+      <c r="M10">
+        <v>16201</v>
+      </c>
+      <c r="N10">
+        <v>17435</v>
+      </c>
+      <c r="O10">
+        <v>17900</v>
+      </c>
+      <c r="P10">
+        <v>24292</v>
+      </c>
+      <c r="Q10">
+        <v>22901</v>
+      </c>
+      <c r="R10">
+        <v>22785</v>
+      </c>
+      <c r="S10">
+        <v>22526</v>
+      </c>
+      <c r="T10">
+        <v>22443</v>
+      </c>
+      <c r="U10">
+        <v>23663</v>
+      </c>
+      <c r="V10">
+        <v>22031</v>
+      </c>
+      <c r="W10">
+        <v>24167</v>
+      </c>
+      <c r="X10">
+        <v>25890</v>
+      </c>
+      <c r="Y10">
+        <v>24594</v>
+      </c>
+      <c r="Z10">
+        <v>26585</v>
+      </c>
+      <c r="AA10">
+        <v>29591</v>
+      </c>
+      <c r="AB10">
+        <v>33234</v>
+      </c>
+      <c r="AC10">
+        <v>33300</v>
+      </c>
+      <c r="AD10">
+        <v>34783</v>
+      </c>
+      <c r="AE10">
+        <v>35181</v>
+      </c>
+      <c r="AF10">
+        <v>34351</v>
+      </c>
+      <c r="AG10">
+        <v>39336</v>
+      </c>
+      <c r="AH10">
+        <v>45122</v>
+      </c>
+      <c r="AI10">
+        <v>58247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>11795</v>
+      </c>
+      <c r="C11">
+        <v>12451</v>
+      </c>
+      <c r="D11">
+        <v>14713</v>
+      </c>
+      <c r="E11">
+        <v>14337</v>
+      </c>
+      <c r="F11">
+        <v>15079</v>
+      </c>
+      <c r="G11">
+        <v>14529</v>
+      </c>
+      <c r="H11">
+        <v>15655</v>
+      </c>
+      <c r="I11">
+        <v>15711</v>
+      </c>
+      <c r="J11">
+        <v>16412</v>
+      </c>
+      <c r="K11">
+        <v>20484</v>
+      </c>
+      <c r="L11">
+        <v>19342</v>
+      </c>
+      <c r="M11">
+        <v>20044</v>
+      </c>
+      <c r="N11">
+        <v>21413</v>
+      </c>
+      <c r="O11">
+        <v>20890</v>
+      </c>
+      <c r="P11">
+        <v>29747</v>
+      </c>
+      <c r="Q11">
+        <v>27976</v>
+      </c>
+      <c r="R11">
+        <v>27809</v>
+      </c>
+      <c r="S11">
+        <v>27394</v>
+      </c>
+      <c r="T11">
+        <v>27244</v>
+      </c>
+      <c r="U11">
+        <v>27826</v>
+      </c>
+      <c r="V11">
+        <v>30118</v>
+      </c>
+      <c r="W11">
+        <v>33225</v>
+      </c>
+      <c r="X11">
+        <v>34299</v>
+      </c>
+      <c r="Y11">
+        <v>35811</v>
+      </c>
+      <c r="Z11">
+        <v>37972</v>
+      </c>
+      <c r="AA11">
+        <v>40306</v>
+      </c>
+      <c r="AB11">
+        <v>47896</v>
+      </c>
+      <c r="AC11">
+        <v>49210</v>
+      </c>
+      <c r="AD11">
+        <v>49869</v>
+      </c>
+      <c r="AE11">
+        <v>48832</v>
+      </c>
+      <c r="AF11">
+        <v>50398</v>
+      </c>
+      <c r="AG11">
+        <v>57055</v>
+      </c>
+      <c r="AH11">
+        <v>66363</v>
+      </c>
+      <c r="AI11">
+        <v>89880</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>15599</v>
+      </c>
+      <c r="C12">
+        <v>16003</v>
+      </c>
+      <c r="D12">
+        <v>18016</v>
+      </c>
+      <c r="E12">
+        <v>17250</v>
+      </c>
+      <c r="F12">
+        <v>17463</v>
+      </c>
+      <c r="G12">
+        <v>16580</v>
+      </c>
+      <c r="H12">
+        <v>19114</v>
+      </c>
+      <c r="I12">
+        <v>18102</v>
+      </c>
+      <c r="J12">
+        <v>17729</v>
+      </c>
+      <c r="K12">
+        <v>18552</v>
+      </c>
+      <c r="L12">
+        <v>17927</v>
+      </c>
+      <c r="M12">
+        <v>16985</v>
+      </c>
+      <c r="N12">
+        <v>18942</v>
+      </c>
+      <c r="O12">
+        <v>20337</v>
+      </c>
+      <c r="P12">
+        <v>21702</v>
+      </c>
+      <c r="Q12">
+        <v>21269</v>
+      </c>
+      <c r="R12">
+        <v>20565</v>
+      </c>
+      <c r="S12">
+        <v>21614</v>
+      </c>
+      <c r="T12">
+        <v>22125</v>
+      </c>
+      <c r="U12">
+        <v>21761</v>
+      </c>
+      <c r="V12">
+        <v>22640</v>
+      </c>
+      <c r="W12">
+        <v>25408</v>
+      </c>
+      <c r="X12">
+        <v>22124</v>
+      </c>
+      <c r="Y12">
+        <v>20275</v>
+      </c>
+      <c r="Z12">
+        <v>22107</v>
+      </c>
+      <c r="AA12">
+        <v>24712</v>
+      </c>
+      <c r="AB12">
+        <v>25701</v>
+      </c>
+      <c r="AC12">
+        <v>25611</v>
+      </c>
+      <c r="AD12">
+        <v>26705</v>
+      </c>
+      <c r="AE12">
+        <v>26032</v>
+      </c>
+      <c r="AF12">
+        <v>26401</v>
+      </c>
+      <c r="AG12">
+        <v>28882</v>
+      </c>
+      <c r="AH12">
+        <v>31104</v>
+      </c>
+      <c r="AI12">
+        <v>38338</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>112</v>
+      </c>
+      <c r="C13">
+        <v>80</v>
+      </c>
+      <c r="D13">
+        <v>77</v>
+      </c>
+      <c r="E13">
+        <v>100</v>
+      </c>
+      <c r="F13">
+        <v>124</v>
+      </c>
+      <c r="G13">
+        <v>117</v>
+      </c>
+      <c r="H13">
+        <v>169</v>
+      </c>
+      <c r="I13">
+        <v>185</v>
+      </c>
+      <c r="J13">
+        <v>146</v>
+      </c>
+      <c r="K13">
+        <v>238</v>
+      </c>
+      <c r="L13">
+        <v>303</v>
+      </c>
+      <c r="M13">
+        <v>313</v>
+      </c>
+      <c r="N13">
+        <v>423</v>
+      </c>
+      <c r="O13">
+        <v>336</v>
+      </c>
+      <c r="P13">
+        <v>399</v>
+      </c>
+      <c r="Q13">
+        <v>421</v>
+      </c>
+      <c r="R13">
+        <v>747</v>
+      </c>
+      <c r="S13">
+        <v>612</v>
+      </c>
+      <c r="T13">
+        <v>609</v>
+      </c>
+      <c r="U13">
+        <v>592</v>
+      </c>
+      <c r="V13">
+        <v>616</v>
+      </c>
+      <c r="W13">
+        <v>600</v>
+      </c>
+      <c r="X13">
+        <v>625</v>
+      </c>
+      <c r="Y13">
+        <v>717</v>
+      </c>
+      <c r="Z13">
+        <v>925</v>
+      </c>
+      <c r="AA13">
+        <v>826</v>
+      </c>
+      <c r="AB13">
+        <v>1065</v>
+      </c>
+      <c r="AC13">
+        <v>1063</v>
+      </c>
+      <c r="AD13">
+        <v>1285</v>
+      </c>
+      <c r="AE13">
+        <v>1323</v>
+      </c>
+      <c r="AF13">
+        <v>1285</v>
+      </c>
+      <c r="AG13">
+        <v>1568</v>
+      </c>
+      <c r="AH13">
+        <v>1755</v>
+      </c>
+      <c r="AI13">
+        <v>2495</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>870</v>
+      </c>
+      <c r="C14">
+        <v>856</v>
+      </c>
+      <c r="D14">
+        <v>865</v>
+      </c>
+      <c r="E14">
+        <v>933</v>
+      </c>
+      <c r="F14">
+        <v>1082</v>
+      </c>
+      <c r="G14">
+        <v>1089</v>
+      </c>
+      <c r="H14">
+        <v>1017</v>
+      </c>
+      <c r="I14">
+        <v>991</v>
+      </c>
+      <c r="J14">
+        <v>1074</v>
+      </c>
+      <c r="K14">
+        <v>1234</v>
+      </c>
+      <c r="L14">
+        <v>1272</v>
+      </c>
+      <c r="M14">
+        <v>1322</v>
+      </c>
+      <c r="N14">
+        <v>1433</v>
+      </c>
+      <c r="O14">
+        <v>1479</v>
+      </c>
+      <c r="P14">
+        <v>1778</v>
+      </c>
+      <c r="Q14">
+        <v>1682</v>
+      </c>
+      <c r="R14">
+        <v>1822</v>
+      </c>
+      <c r="S14">
+        <v>1694</v>
+      </c>
+      <c r="T14">
+        <v>1729</v>
+      </c>
+      <c r="U14">
+        <v>1626</v>
+      </c>
+      <c r="V14">
+        <v>1744</v>
+      </c>
+      <c r="W14">
+        <v>1987</v>
+      </c>
+      <c r="X14">
+        <v>1954</v>
+      </c>
+      <c r="Y14">
+        <v>2106</v>
+      </c>
+      <c r="Z14">
+        <v>2221</v>
+      </c>
+      <c r="AA14">
+        <v>2184</v>
+      </c>
+      <c r="AB14">
+        <v>2575</v>
+      </c>
+      <c r="AC14">
+        <v>2551</v>
+      </c>
+      <c r="AD14">
+        <v>2756</v>
+      </c>
+      <c r="AE14">
+        <v>2772</v>
+      </c>
+      <c r="AF14">
+        <v>2781</v>
+      </c>
+      <c r="AG14">
+        <v>3048</v>
+      </c>
+      <c r="AH14">
+        <v>3619</v>
+      </c>
+      <c r="AI14">
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35">
+      <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="B8">
+      <c r="B15">
         <v>0</v>
       </c>
-      <c r="C8">
+      <c r="C15">
         <v>0</v>
       </c>
-      <c r="D8">
+      <c r="D15">
         <v>0</v>
       </c>
-      <c r="E8">
+      <c r="E15">
         <v>0</v>
       </c>
-      <c r="F8">
+      <c r="F15">
         <v>0</v>
       </c>
-      <c r="G8">
+      <c r="G15">
         <v>1005</v>
       </c>
-      <c r="H8">
+      <c r="H15">
         <v>942</v>
       </c>
-      <c r="I8">
+      <c r="I15">
         <v>1077</v>
       </c>
-      <c r="J8">
+      <c r="J15">
         <v>2343</v>
       </c>
-      <c r="K8">
+      <c r="K15">
         <v>2777</v>
       </c>
-      <c r="L8">
+      <c r="L15">
         <v>2512</v>
       </c>
-      <c r="M8">
+      <c r="M15">
         <v>2344</v>
       </c>
-      <c r="N8">
+      <c r="N15">
         <v>2864</v>
       </c>
-      <c r="O8">
+      <c r="O15">
         <v>3079</v>
       </c>
-      <c r="P8">
+      <c r="P15">
         <v>3699</v>
       </c>
-      <c r="Q8">
+      <c r="Q15">
         <v>4242</v>
       </c>
-      <c r="R8">
+      <c r="R15">
         <v>4252</v>
       </c>
-      <c r="S8">
+      <c r="S15">
         <v>4542</v>
       </c>
-      <c r="T8">
+      <c r="T15">
         <v>4362</v>
       </c>
-      <c r="U8">
+      <c r="U15">
         <v>4376</v>
       </c>
-      <c r="V8">
+      <c r="V15">
         <v>5256</v>
       </c>
-      <c r="W8">
+      <c r="W15">
         <v>6511</v>
       </c>
-      <c r="X8">
+      <c r="X15">
         <v>6753</v>
       </c>
-      <c r="Y8">
+      <c r="Y15">
         <v>7366</v>
       </c>
-      <c r="Z8">
+      <c r="Z15">
         <v>8377</v>
       </c>
-      <c r="AA8">
+      <c r="AA15">
         <v>9948</v>
       </c>
-      <c r="AB8">
+      <c r="AB15">
         <v>10328</v>
       </c>
-      <c r="AC8">
+      <c r="AC15">
         <v>9846</v>
       </c>
-      <c r="AD8">
+      <c r="AD15">
         <v>10042</v>
       </c>
-      <c r="AE8">
+      <c r="AE15">
         <v>10403</v>
       </c>
-      <c r="AF8">
+      <c r="AF15">
         <v>10474</v>
       </c>
-      <c r="AG8">
+      <c r="AG15">
         <v>10832</v>
       </c>
-      <c r="AH8">
+      <c r="AH15">
         <v>13832</v>
       </c>
-      <c r="AI8">
+      <c r="AI15">
         <v>17213</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new lang #6
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -700,7 +700,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -858,11 +857,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2023369816"/>
-        <c:axId val="2023372792"/>
+        <c:axId val="2020305160"/>
+        <c:axId val="2020896936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2023369816"/>
+        <c:axId val="2020305160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -882,7 +881,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2023372792"/>
+        <c:crossAx val="2020896936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -890,7 +889,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2023372792"/>
+        <c:axId val="2020896936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -901,7 +900,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2023369816"/>
+        <c:crossAx val="2020305160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4738,11 +4737,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2108537464"/>
-        <c:axId val="2103510728"/>
+        <c:axId val="2031103352"/>
+        <c:axId val="2031100520"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="2108537464"/>
+        <c:axId val="2031103352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4762,14 +4761,14 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2103510728"/>
+        <c:crossAx val="2031100520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2103510728"/>
+        <c:axId val="2031100520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4780,7 +4779,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108537464"/>
+        <c:crossAx val="2031103352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4817,6 +4816,2013 @@
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup paperSize="9" orientation="portrait" horizontalDpi="-4" verticalDpi="-4"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stats.xlsx.csv!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Clojure</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$1:$AI$1</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>40178.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40209.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40237.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40268.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40298.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40329.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40359.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40390.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40421.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40451.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40482.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40512.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40543.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40574.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40602.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40633.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40663.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40694.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40755.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40786.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40816.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40847.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40877.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40908.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40939.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40968.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40999.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41029.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41060.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41090.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41121.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41152.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41182.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$2:$AI$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>93.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>63.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>78.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>82.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>98.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>89.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>112.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>102.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>118.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>115.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>119.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>135.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>111.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>117.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>112.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>133.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>165.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>223.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>387.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stats.xlsx.csv!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rust</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$1:$AI$1</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>40178.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40209.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40237.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40268.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40298.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40329.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40359.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40390.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40421.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40451.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40482.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40512.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40543.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40574.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40602.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40633.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40663.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40694.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40755.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40786.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40816.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40847.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40877.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40908.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40939.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40968.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40999.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41029.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41060.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41090.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41121.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41152.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41182.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$3:$AI$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>63.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>114.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>74.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>123.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>188.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>206.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>271.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>502.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stats.xlsx.csv!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Haskell</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$1:$AI$1</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>40178.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40209.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40237.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40268.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40298.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40329.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40359.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40390.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40421.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40451.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40482.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40512.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40543.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40574.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40602.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40633.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40663.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40694.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40755.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40786.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40816.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40847.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40877.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40908.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40939.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40968.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40999.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41029.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41060.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41090.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41121.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41152.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41182.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$4:$AI$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>63.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>73.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>73.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>86.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>95.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>69.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>84.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>88.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>81.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>121.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>108.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>124.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>106.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>137.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>135.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>129.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>132.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>112.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>133.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>118.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>138.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>114.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>253.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>259.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>223.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>284.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>333.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>597.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stats.xlsx.csv!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Scala</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$1:$AI$1</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>40178.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40209.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40237.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40268.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40298.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40329.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40359.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40390.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40421.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40451.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40482.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40512.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40543.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40574.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40602.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40633.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40663.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40694.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40755.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40786.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40816.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40847.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40877.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40908.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40939.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40968.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40999.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41029.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41060.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41090.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41121.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41152.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41182.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$5:$AI$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>110.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>85.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>116.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>113.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>117.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>103.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>123.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>117.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>113.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>137.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>131.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>196.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>184.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>163.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>165.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>186.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>198.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>182.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>205.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>134.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>188.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>184.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>214.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>255.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>247.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>280.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>272.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>241.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>306.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>429.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>776.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stats.xlsx.csv!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Perl</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$1:$AI$1</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>40178.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40209.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40237.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40268.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40298.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40329.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40359.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40390.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40421.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40451.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40482.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40512.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40543.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40574.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40602.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40633.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40663.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40694.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40755.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40786.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40816.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40847.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40877.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40908.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40939.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40968.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40999.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41029.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41060.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41090.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41121.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41152.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41182.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$6:$AI$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>145.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>141.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>149.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>141.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>139.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>149.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>145.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>208.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>153.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>176.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>149.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>142.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>190.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>149.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>210.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>173.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>206.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>197.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>161.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>179.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>176.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>255.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>197.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>176.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>219.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>253.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>278.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>298.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>338.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>332.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>441.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>490.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>868.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stats.xlsx.csv!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Swift</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$1:$AI$1</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>40178.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40209.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40237.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40268.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40298.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40329.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40359.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40390.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40421.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40451.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40482.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40512.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40543.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40574.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40602.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40633.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40663.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40694.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40755.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40786.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40816.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40847.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40877.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40908.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40939.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40968.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40999.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41029.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41060.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41090.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41121.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41152.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41182.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$7:$AI$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>131.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>107.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>111.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>145.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>143.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>129.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>131.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>161.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>242.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>240.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>253.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>233.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>264.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>322.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>431.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>343.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>341.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>354.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>415.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>459.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>478.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>451.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>471.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>470.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>556.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1352.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1826.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stats.xlsx.csv!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Objective C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$1:$AI$1</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>40178.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40209.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40237.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40268.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40298.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40329.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40359.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40390.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40421.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40451.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40482.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40512.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40543.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40574.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40602.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40633.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40663.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40694.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40755.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40786.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40816.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40847.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40877.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40908.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40939.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40968.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40999.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41029.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41060.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41090.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41121.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41152.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41182.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$8:$AI$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>611.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>578.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>659.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>686.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>664.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>535.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>580.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>588.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>533.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>533.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>543.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>586.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>523.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>706.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>734.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>727.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>702.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>805.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>899.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>812.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>883.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>762.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>904.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1010.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1155.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1127.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1070.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1100.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1103.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1131.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1283.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1564.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1966.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stats.xlsx.csv!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Go</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$1:$AI$1</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>40178.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40209.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40237.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40268.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40298.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40329.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40359.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40390.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40421.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40451.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40482.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40512.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40543.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40574.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40602.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40633.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40663.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40694.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40724.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40755.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40786.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40816.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40847.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40877.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40908.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40939.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40968.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40999.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41029.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41060.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41090.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41121.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41152.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41182.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stats.xlsx.csv!$B$9:$AI$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>202.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>210.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>227.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>217.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>258.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>248.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>284.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>295.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>301.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>304.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>295.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>362.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>432.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>356.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>463.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>427.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>438.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>439.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>479.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>520.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>527.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>567.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>432.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>385.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>511.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>511.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>701.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>633.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>693.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>715.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>767.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1086.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1341.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2189.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2100305496"/>
+        <c:axId val="2114895928"/>
+      </c:areaChart>
+      <c:dateAx>
+        <c:axId val="2100305496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="[$-409]mmm\-yy;@" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1"/>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2114895928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="2114895928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2100305496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.833812113108503"/>
+          <c:y val="0.0197184222939874"/>
+          <c:w val="0.156124993809736"/>
+          <c:h val="0.975924138514944"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="1"/>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -4883,6 +6889,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4891,11 +6927,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2015" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2016" connectionId="9" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2016" connectionId="9" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2015" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5222,8 +7258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="AB66" sqref="AB66"/>
+    <sheetView tabSelected="1" topLeftCell="J20" workbookViewId="0">
+      <selection sqref="A1:AI9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>